<commit_message>
update 10 thang 1 nam 2024
</commit_message>
<xml_diff>
--- a/src/test/resources/dataTest/Login.xlsx
+++ b/src/test/resources/dataTest/Login.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NguyenVanPhuc\src\test\resources\dataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F5D04C-BB51-422E-B932-61108E1B9132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7AF62D-2765-4B30-85BC-69A0578FD484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CD1A626E-987F-458F-BC2F-30662875B4EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{CD1A626E-987F-458F-BC2F-30662875B4EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="DataLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>email</t>
   </si>
@@ -45,6 +46,12 @@
   </si>
   <si>
     <t>admin@example.com</t>
+  </si>
+  <si>
+    <t>admin1@example.com</t>
+  </si>
+  <si>
+    <t>admin11@example.com</t>
   </si>
 </sst>
 </file>
@@ -80,9 +87,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C1A16A-861D-4422-A50D-067B079AE28B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,7 +423,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
@@ -425,7 +431,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -433,7 +439,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -441,7 +447,66 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>123456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB280D7C-958A-4C44-8716-24224DEC03C3}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">

</xml_diff>

<commit_message>
update capture and record
</commit_message>
<xml_diff>
--- a/src/test/resources/dataTest/Login.xlsx
+++ b/src/test/resources/dataTest/Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NguyenVanPhuc\src\test\resources\dataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7AF62D-2765-4B30-85BC-69A0578FD484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5509F9AE-93F3-4124-BD6C-EEB9D2580DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{CD1A626E-987F-458F-BC2F-30662875B4EA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
     <t>email</t>
   </si>
@@ -48,10 +48,7 @@
     <t>admin@example.com</t>
   </si>
   <si>
-    <t>admin1@example.com</t>
-  </si>
-  <si>
-    <t>admin11@example.com</t>
+    <t>123456</t>
   </si>
 </sst>
 </file>
@@ -87,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB280D7C-958A-4C44-8716-24224DEC03C3}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,32 +483,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B4">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>123456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>